<commit_message>
Atualização do Roteiro de Testes
</commit_message>
<xml_diff>
--- a/CHP/4.Teste/CHP - Roteiro de Teste.xlsx
+++ b/CHP/4.Teste/CHP - Roteiro de Teste.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Alonso\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\CHP\chamado-pro\CHP\4.Teste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB592AD9-2099-4872-8343-F841FB940F8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="913" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="913" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -26,13 +25,13 @@
     <definedName name="__xlfn_IFERROR">NA()</definedName>
     <definedName name="combo_SimNao">AUX!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -128,16 +127,25 @@
   </si>
   <si>
     <t>&lt;UC Fazer Login&gt;</t>
+  </si>
+  <si>
+    <t>Manter Chamado</t>
+  </si>
+  <si>
+    <t>A massa de teste está disponível em...</t>
+  </si>
+  <si>
+    <t>resultado esperado no sistema, exemplo: "Erro, digite no nome"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-416]General"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -329,6 +337,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="17">
@@ -747,7 +763,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -839,24 +855,27 @@
     <xf numFmtId="0" fontId="23" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="16">
-    <cellStyle name="Bad" xfId="5" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Bom" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Calculation" xfId="2" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Excel Built-in Normal" xfId="15" xr:uid="{5BABCF39-029E-4523-A85E-C39043BF46AE}"/>
-    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="4" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Bom" xfId="1"/>
+    <cellStyle name="Cálculo" xfId="2" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula de Verificação" xfId="3"/>
+    <cellStyle name="Entrada" xfId="4" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Excel Built-in Normal" xfId="15"/>
+    <cellStyle name="Incorreto" xfId="5" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutra" xfId="6"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Note" xfId="8" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Porcentagem 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Título 5" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 3" xfId="7"/>
+    <cellStyle name="Nota" xfId="8" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Porcentagem 2" xfId="9"/>
+    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="11" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título 5" xfId="13"/>
     <cellStyle name="Total" xfId="14" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="11" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1286,7 +1305,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L22"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
@@ -1560,7 +1579,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1597,12 +1616,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1625,7 +1644,7 @@
     </row>
     <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
       <c r="A2" s="35">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B2" s="35"/>
       <c r="C2" s="35"/>
@@ -1633,6 +1652,272 @@
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
         <v>28</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="39"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>6</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>9</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>10</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>11</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="35">
+        <v>6</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>29</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -1854,8 +2139,267 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+    </row>
+    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
+      <c r="A2" s="35">
+        <v>6</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="38"/>
+      <c r="C4" s="15"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="15"/>
+    </row>
+    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>2</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+      <c r="W10" s="5"/>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>3</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>4</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10">
+        <v>6</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>7</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>8</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>9</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>10</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="10">
+        <v>11</v>
+      </c>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:B4"/>
+  </mergeCells>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter alignWithMargins="0">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1891,7 +2435,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -2113,13 +2657,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7219EEEA-3919-48A4-ABBD-4770C1FFC26D}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2150,7 +2694,7 @@
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -2370,522 +2914,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703DFFD6-BFA4-4B9B-BD1C-773517DB4051}">
-  <dimension ref="A1:W19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-    </row>
-    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
-        <v>6</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-    </row>
-    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-    </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="15"/>
-    </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-    </row>
-    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>2</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-    </row>
-    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:B4"/>
-  </mergeCells>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8368203-C6FE-4148-9F0C-6012F80C7C5D}">
-  <dimension ref="A1:W19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="39.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-    </row>
-    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
-        <v>6</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-    </row>
-    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-    </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="15"/>
-    </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-    </row>
-    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
-        <v>2</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="5"/>
-      <c r="W10" s="5"/>
-    </row>
-    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
-  </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:B4"/>
-  </mergeCells>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
alteração no guia de implementação e testes.
</commit_message>
<xml_diff>
--- a/CHP/4.Teste/CHP - Roteiro de Teste.xlsx
+++ b/CHP/4.Teste/CHP - Roteiro de Teste.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aluno\Desktop\CHP\chamado-pro\CHP\4.Teste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Alonso\Desktop\CHP\chamado-pro\CHP\4.Teste\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8F6F59-C831-4E0B-A779-61F7C97626E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="913" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="913" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capa" sheetId="1" r:id="rId1"/>
@@ -25,13 +26,13 @@
     <definedName name="__xlfn_IFERROR">NA()</definedName>
     <definedName name="combo_SimNao">AUX!$A$2:$A$3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
   <si>
     <t>Caso de Uso</t>
   </si>
@@ -132,16 +133,142 @@
     <t>Manter Chamado</t>
   </si>
   <si>
-    <t>A massa de teste está disponível em...</t>
-  </si>
-  <si>
-    <t>resultado esperado no sistema, exemplo: "Erro, digite no nome"</t>
+    <t>acesso com senha inválida</t>
+  </si>
+  <si>
+    <t>acesso email inválido</t>
+  </si>
+  <si>
+    <t>acesso com senha e email inválidos</t>
+  </si>
+  <si>
+    <t>acesso com senha e email válidos</t>
+  </si>
+  <si>
+    <t>acessar com senha inválida, mas email válido</t>
+  </si>
+  <si>
+    <t>acessar com email inválido, mas senha válida</t>
+  </si>
+  <si>
+    <t>acesso com todos os dados de login corretos</t>
+  </si>
+  <si>
+    <t>acesso com todos os dados de login incorretos</t>
+  </si>
+  <si>
+    <t>"Email ou senha incorretos!"</t>
+  </si>
+  <si>
+    <t>acesso ao sistema</t>
+  </si>
+  <si>
+    <t>"clicar" no botão "detalhes"</t>
+  </si>
+  <si>
+    <t>detalhes do chamado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">editar chamado </t>
+  </si>
+  <si>
+    <t>nome do chamado e descrição</t>
+  </si>
+  <si>
+    <t>excluir chamado</t>
+  </si>
+  <si>
+    <t>"clicar" no botão "excluir" e selecionar "ok" na mensagem de confirmação</t>
+  </si>
+  <si>
+    <t>Email ou senha incorretos!</t>
+  </si>
+  <si>
+    <t>todos os chamados abertos na tela</t>
+  </si>
+  <si>
+    <t>lista de todos os chamados abertos ao acessar a tela "chamados"</t>
+  </si>
+  <si>
+    <t>criar chamado</t>
+  </si>
+  <si>
+    <t>titulo e descrição</t>
+  </si>
+  <si>
+    <t>mensagem "Chamado atualizado com sucesso!", com os dados atualizados na tela de "chamados"</t>
+  </si>
+  <si>
+    <t>criar usuário</t>
+  </si>
+  <si>
+    <t>nome, email, senha, tipo de usuário</t>
+  </si>
+  <si>
+    <t>mensagem "Usuário criado com sucesso!", usuário na lista de chamados e acesso ao sistema com novo usuário</t>
+  </si>
+  <si>
+    <t>editar usuário</t>
+  </si>
+  <si>
+    <t>nome e email</t>
+  </si>
+  <si>
+    <t>dados atualizados do usuário na lista de usuários</t>
+  </si>
+  <si>
+    <t>excluir usuário</t>
+  </si>
+  <si>
+    <t>"clicar" em "deletar" e selecionar "ok" na mensagem de confirmação</t>
+  </si>
+  <si>
+    <t>usuário deletado do sistema</t>
+  </si>
+  <si>
+    <t>mensagem "Chamado criado com sucesso!" e chamado listado na tela "chamados"</t>
+  </si>
+  <si>
+    <t>mensagem "chamado excluído com sucesso!" e chamado excluido da lista de chamados</t>
+  </si>
+  <si>
+    <t>A massa de teste está disponível em: https://github.com/guualonso/chamado-pro/blob/develop/CHP/4.Teste</t>
+  </si>
+  <si>
+    <t>O usuário deve estar logado no Sistema, possuir perfil de acesso à funcionalidade e necessário haver chamados abertos .</t>
+  </si>
+  <si>
+    <t>O usuário deve ter cadastro no sistema .</t>
+  </si>
+  <si>
+    <t>consulta de chamados abertos</t>
+  </si>
+  <si>
+    <t>criação, edição e exclusão de usuários</t>
+  </si>
+  <si>
+    <t>acessar o sistema com um usuário cadastrado</t>
+  </si>
+  <si>
+    <t>fazer comentário</t>
+  </si>
+  <si>
+    <t>criação do comentário no chamado</t>
+  </si>
+  <si>
+    <t>"comentário: teste"</t>
+  </si>
+  <si>
+    <t>visualizar comentário</t>
+  </si>
+  <si>
+    <t>visualização do comentário</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-416]General"/>
   </numFmts>
@@ -445,7 +572,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -744,6 +871,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -763,7 +903,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -834,6 +974,36 @@
     <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="27" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -841,6 +1011,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -855,27 +1040,36 @@
     <xf numFmtId="0" fontId="23" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
-    <cellStyle name="Bom" xfId="1"/>
-    <cellStyle name="Cálculo" xfId="2" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="3"/>
-    <cellStyle name="Entrada" xfId="4" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Excel Built-in Normal" xfId="15"/>
-    <cellStyle name="Incorreto" xfId="5" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="6"/>
+    <cellStyle name="Bad" xfId="5" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Bom" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Calculation" xfId="2" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula de Verificação" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="4" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Neutra" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="7"/>
-    <cellStyle name="Nota" xfId="8" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Porcentagem 2" xfId="9"/>
-    <cellStyle name="Saída" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de Aviso" xfId="11" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto Explicativo" xfId="12" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título 5" xfId="13"/>
+    <cellStyle name="Normal 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Note" xfId="8" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Porcentagem 2" xfId="9" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Título 5" xfId="13" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
     <cellStyle name="Total" xfId="14" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="11" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1305,11 +1499,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L22"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1331,18 +1525,18 @@
     <row r="1" spans="2:12" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="24"/>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="33"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="43"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B3" s="25"/>
@@ -1375,8 +1569,12 @@
       <c r="C5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="22"/>
-      <c r="F5" s="20"/>
+      <c r="D5" s="22">
+        <v>3</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0</v>
+      </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
       <c r="L5" s="26"/>
@@ -1386,8 +1584,12 @@
       <c r="C6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="22"/>
-      <c r="F6" s="20"/>
+      <c r="D6" s="22">
+        <v>2</v>
+      </c>
+      <c r="F6" s="20">
+        <v>0</v>
+      </c>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
       <c r="L6" s="26"/>
@@ -1397,8 +1599,12 @@
       <c r="C7" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="F7" s="20"/>
+      <c r="D7" s="22">
+        <v>3</v>
+      </c>
+      <c r="F7" s="20">
+        <v>0</v>
+      </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
       <c r="L7" s="26"/>
@@ -1408,8 +1614,12 @@
       <c r="C8" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="F8" s="20"/>
+      <c r="D8" s="22">
+        <v>4</v>
+      </c>
+      <c r="F8" s="20">
+        <v>0</v>
+      </c>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="L8" s="26"/>
@@ -1534,7 +1744,7 @@
       </c>
       <c r="D21" s="22">
         <f>SUM(D5:D19)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F21" s="3">
         <f>SUM(F5:F19)</f>
@@ -1579,7 +1789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1616,12 +1826,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1635,45 +1845,64 @@
     <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-    </row>
-    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
-        <v>11</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-    </row>
-    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+    </row>
+    <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="45">
+        <v>3</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-    </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="48"/>
+      <c r="C4" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="39"/>
-    </row>
-    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="D4" s="34"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+    </row>
+    <row r="5" spans="1:23" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A5" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
@@ -1683,43 +1912,61 @@
       <c r="C6" s="16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+    </row>
+    <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="32"/>
+      <c r="B7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="32"/>
+      <c r="G7" s="32"/>
+    </row>
+    <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="37" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
+    <row r="9" spans="1:23" ht="57" x14ac:dyDescent="0.2">
+      <c r="A9" s="38">
         <v>1</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11" t="s">
-        <v>34</v>
+      <c r="B9" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="39" t="s">
+        <v>64</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -1737,16 +1984,24 @@
       <c r="V9" s="5"/>
       <c r="W9" s="5"/>
     </row>
-    <row r="10" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9">
+    <row r="10" spans="1:23" ht="57" x14ac:dyDescent="0.2">
+      <c r="A10" s="40">
         <v>2</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>54</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -1764,105 +2019,28 @@
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
     </row>
-    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
+    <row r="11" spans="1:23" ht="57" x14ac:dyDescent="0.2">
+      <c r="A11" s="40">
         <v>3</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>65</v>
+      </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
+      <c r="G11" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="4">
@@ -1881,12 +2059,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1902,48 +2080,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
-        <v>6</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="A2" s="50">
+        <v>2</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
     </row>
     <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="15" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="15"/>
+      <c r="C5" s="55" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="16" t="s">
-        <v>14</v>
-      </c>
+      <c r="C6" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="54"/>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1973,12 +2158,18 @@
       <c r="A9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="11"/>
+      <c r="B9" s="11" t="s">
+        <v>51</v>
+      </c>
       <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="D9" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -2000,12 +2191,20 @@
       <c r="A10" s="9">
         <v>2</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>44</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -2023,112 +2222,18 @@
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
     </row>
-    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
+    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C6:F6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2140,12 +2245,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2161,48 +2266,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
-        <v>6</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="A2" s="50">
+        <v>3</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
     </row>
     <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="15" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="15"/>
+      <c r="C5" s="55" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="54" t="s">
         <v>14</v>
       </c>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2232,12 +2343,20 @@
       <c r="A9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="B9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>57</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -2259,12 +2378,20 @@
       <c r="A10" s="9">
         <v>2</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -2286,108 +2413,32 @@
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
+      <c r="G11" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2399,19 +2450,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="74.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="4" bestFit="1" customWidth="1"/>
@@ -2420,47 +2471,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
-        <v>6</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="A2" s="50">
+        <v>4</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-    </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+    </row>
+    <row r="4" spans="1:23" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="53"/>
+      <c r="C4" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="15"/>
-    </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8"/>
       <c r="C6" s="16" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2491,12 +2546,20 @@
       <c r="A9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="B9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>41</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -2518,12 +2581,20 @@
       <c r="A10" s="9">
         <v>2</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>49</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -2545,101 +2616,42 @@
       <c r="A11" s="9">
         <v>3</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
+      <c r="G11" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>4</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+      <c r="B12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>42</v>
+      </c>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
+      <c r="G12" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="4">
@@ -2658,19 +2670,19 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.140625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" style="4" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="38.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="4" bestFit="1" customWidth="1"/>
@@ -2679,48 +2691,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:23" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
-        <v>6</v>
-      </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
+      <c r="A2" s="50">
+        <v>2</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
     </row>
     <row r="3" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-    </row>
-    <row r="4" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="37" t="s">
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+    </row>
+    <row r="4" spans="1:23" ht="29.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="15"/>
-    </row>
-    <row r="5" spans="1:23" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="53"/>
+      <c r="C4" s="15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="7"/>
-      <c r="C5" s="15"/>
-    </row>
-    <row r="6" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="54" t="s">
         <v>14</v>
       </c>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
     </row>
     <row r="7" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="8" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2746,16 +2764,24 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:23" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="10">
         <v>1</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="B9" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="56" t="s">
+        <v>73</v>
+      </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
+      <c r="G9" s="13">
+        <v>1</v>
+      </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -2777,12 +2803,18 @@
       <c r="A10" s="9">
         <v>2</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+      <c r="B10" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57" t="s">
+        <v>76</v>
+      </c>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
+      <c r="G10" s="13">
+        <v>1</v>
+      </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -2800,112 +2832,18 @@
       <c r="V10" s="5"/>
       <c r="W10" s="5"/>
     </row>
-    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-    </row>
-    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10">
-        <v>6</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A15" s="9">
-        <v>7</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-    </row>
-    <row r="16" spans="1:23" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="9">
-        <v>8</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="9">
-        <v>9</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="9">
-        <v>10</v>
-      </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10">
-        <v>11</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-    </row>
+    <row r="11" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:23" ht="16.5" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C6:E6"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>